<commit_message>
Finished grading weeks 2 and 3
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="166" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="121">
   <si>
     <t>Tutorial_01_1</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>Program_12_3</t>
+  </si>
+  <si>
+    <t>Failed to run</t>
+  </si>
+  <si>
+    <t>Does not run</t>
   </si>
 </sst>
 </file>
@@ -1553,9 +1559,9 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="8" style="16" customWidth="true"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="46" customWidth="true"/>
+    <col min="4" max="4" width="6.7109375" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1574,31 +1580,55 @@
       <c r="A2" t="s">
         <v>85</v>
       </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>87</v>
       </c>
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1615,9 +1645,9 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="9.1640625" style="16" customWidth="true"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="46" customWidth="true"/>
+    <col min="4" max="4" width="13.140625" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1636,55 +1666,103 @@
       <c r="A2" t="s">
         <v>95</v>
       </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>96</v>
       </c>
+      <c r="B3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>97</v>
       </c>
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>100</v>
       </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>101</v>
       </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>102</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding grades for week 5
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="168" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="169" uniqueCount="121">
   <si>
     <t>Tutorial_01_1</t>
   </si>
@@ -1837,9 +1837,9 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="10.83203125" style="16"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="46" customWidth="true"/>
+    <col min="4" max="4" width="13.140625" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1858,56 +1858,102 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>66</v>
       </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>67</v>
       </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>63</v>
       </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>64</v>
       </c>
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Added grades for weeks 6 and 7
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="170" uniqueCount="122">
   <si>
     <t>Tutorial_01_1</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>Does not run</t>
+  </si>
+  <si>
+    <t>Just a tip, usually you would validate the input before performing any action. Also, though I haven't tested it, I think there is a minor bug in your gridOn code. I think that if you don't supply a gridOn parameter, this will call gridOff since you don't have else with the exist condition. Obviously no points off, just thought you might want some pointers. Kudos on using the short-circuit AND.</t>
   </si>
 </sst>
 </file>
@@ -1970,9 +1973,9 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="12.6640625" style="16" customWidth="true"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="46" customWidth="true"/>
+    <col min="4" max="4" width="6.7109375" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1991,26 +1994,46 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2027,9 +2050,9 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="10.83203125" style="16"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="46" customWidth="true"/>
+    <col min="4" max="4" width="358.140625" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -2048,66 +2071,120 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>68</v>
       </c>
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0"/>
     </row>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>70</v>
       </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>